<commit_message>
Added gantt chart to semester report
</commit_message>
<xml_diff>
--- a/First Semester Report/Gantt Chart.xlsx
+++ b/First Semester Report/Gantt Chart.xlsx
@@ -332,6 +332,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -340,12 +346,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -542,10 +542,10 @@
                   <c:v>43353</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43364</c:v>
+                  <c:v>43366</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43364</c:v>
+                  <c:v>43366</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>43388</c:v>
@@ -1518,7 +1518,7 @@
                   <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -2266,13 +2266,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>253999</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>65809</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>136070</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>277091</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2652,8 +2652,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:V53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2674,24 +2674,24 @@
   <sheetData>
     <row r="1" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:22" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
@@ -2748,15 +2748,15 @@
         <f>C5</f>
         <v>43297</v>
       </c>
-      <c r="M4" s="28" t="s">
+      <c r="M4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
     </row>
     <row r="5" spans="2:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
@@ -3181,11 +3181,11 @@
         <v>23</v>
       </c>
       <c r="C21" s="9">
-        <v>43364</v>
+        <v>43366</v>
       </c>
       <c r="D21" s="18">
         <f t="shared" si="2"/>
-        <v>43403</v>
+        <v>43405</v>
       </c>
       <c r="E21" s="10">
         <v>40</v>
@@ -3207,11 +3207,11 @@
         <v>31</v>
       </c>
       <c r="C22" s="3">
-        <v>43364</v>
+        <v>43366</v>
       </c>
       <c r="D22" s="18">
         <f t="shared" si="2"/>
-        <v>43403</v>
+        <v>43405</v>
       </c>
       <c r="E22" s="6">
         <v>40</v>
@@ -3237,10 +3237,10 @@
       </c>
       <c r="D23" s="18">
         <f t="shared" si="2"/>
-        <v>43399</v>
+        <v>43405</v>
       </c>
       <c r="E23" s="6">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F23" s="19">
         <f t="shared" si="0"/>
@@ -3248,7 +3248,7 @@
       </c>
       <c r="G23" s="19">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H23" s="7">
         <v>0</v>
@@ -3258,7 +3258,7 @@
       <c r="B24" s="21"/>
       <c r="C24" s="3"/>
       <c r="D24" s="18" t="str">
-        <f t="shared" ref="D5:D29" si="3">IF(ISBLANK(E24),"",E24+C24)</f>
+        <f t="shared" ref="D24:D29" si="3">IF(ISBLANK(E24),"",E24+C24)</f>
         <v/>
       </c>
       <c r="E24" s="6"/>
@@ -3382,18 +3382,18 @@
       <c r="J31" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="K31" s="24" t="s">
+      <c r="K31" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
-      <c r="O31" s="24"/>
-      <c r="P31" s="26" t="s">
+      <c r="L31" s="26"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="26"/>
+      <c r="O31" s="26"/>
+      <c r="P31" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="Q31" s="26"/>
-      <c r="R31" s="26"/>
+      <c r="Q31" s="28"/>
+      <c r="R31" s="28"/>
     </row>
     <row r="32" spans="2:18" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="13"/>
@@ -3403,18 +3403,18 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
-      <c r="K32" s="25" t="s">
+      <c r="K32" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="L32" s="25"/>
-      <c r="M32" s="25"/>
-      <c r="N32" s="25"/>
-      <c r="O32" s="25"/>
-      <c r="P32" s="25" t="s">
+      <c r="L32" s="27"/>
+      <c r="M32" s="27"/>
+      <c r="N32" s="27"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="Q32" s="25"/>
-      <c r="R32" s="25"/>
+      <c r="Q32" s="27"/>
+      <c r="R32" s="27"/>
     </row>
     <row r="33" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="13"/>

</xml_diff>

<commit_message>
Finished gantt chart in excel sheet
</commit_message>
<xml_diff>
--- a/First Semester Report/Gantt Chart.xlsx
+++ b/First Semester Report/Gantt Chart.xlsx
@@ -110,12 +110,6 @@
     <t>Implement Neural Network on a Sensor Node</t>
   </si>
   <si>
-    <t>Implement and Train Neural Network on PC Using Sensor Data</t>
-  </si>
-  <si>
-    <t>Design and Implement and Simulate Neural Network on PC Using Dummy Data</t>
-  </si>
-  <si>
     <t>Background Study on Feed-Forward Neural Networks</t>
   </si>
   <si>
@@ -126,6 +120,12 @@
   </si>
   <si>
     <t>Practice Oral for Final Exam</t>
+  </si>
+  <si>
+    <t>Design and Implement and Simulate Neural Network</t>
+  </si>
+  <si>
+    <t>Implement and Train Neural Network on PC</t>
   </si>
 </sst>
 </file>
@@ -461,10 +461,10 @@
                   <c:v>Background Study on Neural Network Trainnig Methods</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Design and Implement and Simulate Neural Network on PC Using Dummy Data</c:v>
+                  <c:v>Design and Implement and Simulate Neural Network</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Implement and Train Neural Network on PC Using Sensor Data</c:v>
+                  <c:v>Implement and Train Neural Network on PC</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Implement Neural Network on a Sensor Node</c:v>
@@ -937,10 +937,10 @@
                   <c:v>Background Study on Neural Network Trainnig Methods</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Design and Implement and Simulate Neural Network on PC Using Dummy Data</c:v>
+                  <c:v>Design and Implement and Simulate Neural Network</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Implement and Train Neural Network on PC Using Sensor Data</c:v>
+                  <c:v>Implement and Train Neural Network on PC</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Implement Neural Network on a Sensor Node</c:v>
@@ -1431,10 +1431,10 @@
                   <c:v>Background Study on Neural Network Trainnig Methods</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Design and Implement and Simulate Neural Network on PC Using Dummy Data</c:v>
+                  <c:v>Design and Implement and Simulate Neural Network</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Implement and Train Neural Network on PC Using Sensor Data</c:v>
+                  <c:v>Implement and Train Neural Network on PC</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Implement Neural Network on a Sensor Node</c:v>
@@ -1589,7 +1589,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1615,7 +1615,7 @@
         <c:axId val="-2095144704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="43418"/>
+          <c:max val="43410"/>
           <c:min val="43297"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1634,7 +1634,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="0"/>
+        <c:numFmt formatCode="d/m" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1652,7 +1652,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2269,8 +2269,8 @@
       <xdr:rowOff>65809</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>136070</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>326571</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>277091</xdr:rowOff>
     </xdr:to>
@@ -2652,8 +2652,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:V53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2995,7 +2995,7 @@
     </row>
     <row r="14" spans="2:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" s="3">
         <v>43325</v>
@@ -3021,7 +3021,7 @@
     </row>
     <row r="15" spans="2:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" s="3">
         <v>43325</v>
@@ -3047,7 +3047,7 @@
     </row>
     <row r="16" spans="2:22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="21" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C16" s="3">
         <v>43332</v>
@@ -3074,7 +3074,7 @@
     </row>
     <row r="17" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C17" s="3">
         <v>43339</v>
@@ -3204,7 +3204,7 @@
     </row>
     <row r="22" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C22" s="3">
         <v>43366</v>
@@ -3230,7 +3230,7 @@
     </row>
     <row r="23" spans="2:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C23" s="3">
         <v>43388</v>

</xml_diff>